<commit_message>
Added Excel reader, writer, Implemented several other functions and Methods
</commit_message>
<xml_diff>
--- a/LetsTestATP/LetsTestATP/Datasheets/LoginInfo.xlsx
+++ b/LetsTestATP/LetsTestATP/Datasheets/LoginInfo.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="600" windowWidth="21570" windowHeight="9255"/>
+    <workbookView xWindow="0" yWindow="1200" windowWidth="21570" windowHeight="9255"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,9 +26,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>Login</t>
-  </si>
-  <si>
     <t>Password</t>
   </si>
   <si>
@@ -36,6 +33,9 @@
   </si>
   <si>
     <t>Fail1234</t>
+  </si>
+  <si>
+    <t>Username</t>
   </si>
 </sst>
 </file>
@@ -390,25 +390,25 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Separated Excel Reader to separate test case.
</commit_message>
<xml_diff>
--- a/LetsTestATP/LetsTestATP/Datasheets/LoginInfo.xlsx
+++ b/LetsTestATP/LetsTestATP/Datasheets/LoginInfo.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1200" windowWidth="21570" windowHeight="9255"/>
+    <workbookView xWindow="0" yWindow="1800" windowWidth="21570" windowHeight="9255"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="14">
   <si>
     <t>Password</t>
   </si>
@@ -36,6 +36,36 @@
   </si>
   <si>
     <t>Username</t>
+  </si>
+  <si>
+    <t>Role</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>Fail1235</t>
+  </si>
+  <si>
+    <t>Fail1236</t>
+  </si>
+  <si>
+    <t>Fail1237</t>
+  </si>
+  <si>
+    <t>Fail1238</t>
+  </si>
+  <si>
+    <t>Fail1239</t>
+  </si>
+  <si>
+    <t>Fail1240</t>
+  </si>
+  <si>
+    <t>Fail1241</t>
+  </si>
+  <si>
+    <t>Fail1242</t>
   </si>
 </sst>
 </file>
@@ -387,28 +417,122 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>